<commit_message>
I have now updated the database with all the dummy information. I will now do one final check of the database and attempt to build it.
</commit_message>
<xml_diff>
--- a/Entity Relationship Diagram/Database Data/Dummy Data.xlsx
+++ b/Entity Relationship Diagram/Database Data/Dummy Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Blnkspc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepos\circle_lab_project\Entity Relationship Diagram\Database Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B50322-5A2D-4386-BAFD-1A56198F659F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C224EAC7-60CD-4D8D-93DB-0DD5FA4778D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="6435" windowWidth="21600" windowHeight="11385" xr2:uid="{AED28F28-28A4-49FA-98A9-4DD437F4C446}"/>
+    <workbookView xWindow="4680" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{AED28F28-28A4-49FA-98A9-4DD437F4C446}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
   <si>
     <t>Symptoms</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Disease</t>
   </si>
   <si>
-    <t xml:space="preserve">Causes </t>
-  </si>
-  <si>
     <t>Treatments</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Broken ankle </t>
   </si>
   <si>
-    <t xml:space="preserve">injury </t>
-  </si>
-  <si>
     <t>painkiller</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>Heel pain</t>
   </si>
   <si>
-    <t>band of tissue in the foot becomes damaged and thickens</t>
-  </si>
-  <si>
     <t>resting your heel</t>
   </si>
   <si>
@@ -137,9 +128,6 @@
     <t>Oedema </t>
   </si>
   <si>
-    <t>pregnancy</t>
-  </si>
-  <si>
     <t>losing weight </t>
   </si>
   <si>
@@ -149,9 +137,6 @@
     <t>pitting oedema</t>
   </si>
   <si>
-    <t>kidney disease </t>
-  </si>
-  <si>
     <t>taking regular exercise </t>
   </si>
   <si>
@@ -161,9 +146,6 @@
     <t>aching, tender limbs</t>
   </si>
   <si>
-    <t>heart failure </t>
-  </si>
-  <si>
     <t>raising your legs three to four times a day</t>
   </si>
   <si>
@@ -173,39 +155,18 @@
     <t>stiff joints</t>
   </si>
   <si>
-    <t>chronic lung disease </t>
-  </si>
-  <si>
     <t>avoiding standing for long periods of time</t>
   </si>
   <si>
     <t>weight gain</t>
   </si>
   <si>
-    <t>thyroid disease</t>
-  </si>
-  <si>
-    <t>liver disease  </t>
-  </si>
-  <si>
-    <t>malnutrition</t>
-  </si>
-  <si>
-    <t>medication</t>
-  </si>
-  <si>
-    <t>the contraceptive pill</t>
-  </si>
-  <si>
     <t>"creepy-crawly" feeling</t>
   </si>
   <si>
     <t>Restless legs syndrome </t>
   </si>
   <si>
-    <t xml:space="preserve">unknown </t>
-  </si>
-  <si>
     <t>lifestyle changes</t>
   </si>
   <si>
@@ -239,9 +200,6 @@
     <t>Sprains and strains </t>
   </si>
   <si>
-    <t>overreach</t>
-  </si>
-  <si>
     <t>PRICE therapy</t>
   </si>
   <si>
@@ -251,9 +209,6 @@
     <t>inability to put weight on it</t>
   </si>
   <si>
-    <t>change direction or speed suddenly</t>
-  </si>
-  <si>
     <t>Avoiding HARM</t>
   </si>
   <si>
@@ -263,18 +218,12 @@
     <t>swelling</t>
   </si>
   <si>
-    <t>fall and land awkwardly</t>
-  </si>
-  <si>
     <t>painkillers</t>
   </si>
   <si>
     <t>inability to use the joint normally</t>
   </si>
   <si>
-    <t>collide with an object or person</t>
-  </si>
-  <si>
     <t>Physiotherapy</t>
   </si>
   <si>
@@ -299,9 +248,6 @@
     <t>Varicose eczema </t>
   </si>
   <si>
-    <t>increased pressure in the leg veins</t>
-  </si>
-  <si>
     <t>self-help measures</t>
   </si>
   <si>
@@ -353,36 +299,21 @@
     <t>a build-up of fluid around the knee</t>
   </si>
   <si>
-    <t>blow to the knee </t>
-  </si>
-  <si>
     <t>ice pack</t>
   </si>
   <si>
     <t>occasional locking or clicking in the knee joint</t>
   </si>
   <si>
-    <t>osteoarthritis</t>
-  </si>
-  <si>
     <t>pain in the knee</t>
   </si>
   <si>
-    <t>inflammatory arthritis</t>
-  </si>
-  <si>
-    <t>gout</t>
-  </si>
-  <si>
     <t>severely painful leg</t>
   </si>
   <si>
     <t>Broken leg</t>
   </si>
   <si>
-    <t>injury</t>
-  </si>
-  <si>
     <t>Immobilisation</t>
   </si>
   <si>
@@ -413,9 +344,6 @@
     <t>Charcot-Marie-Tooth disease </t>
   </si>
   <si>
-    <t>genes </t>
-  </si>
-  <si>
     <t>physiotherapy </t>
   </si>
   <si>
@@ -450,9 +378,6 @@
   </si>
   <si>
     <t>Deep vein thrombosis </t>
-  </si>
-  <si>
-    <t>age</t>
   </si>
   <si>
     <t>anticoagulant medicines</t>
@@ -874,22 +799,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528E7105-FF1C-4147-B82E-CE0932820990}">
-  <dimension ref="A1:E79"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E80"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -902,769 +826,647 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D28" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C46" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B59" s="1"/>
-      <c r="C59" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="D63" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>121</v>
+        <v>98</v>
       </c>
       <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="D64" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D46" r:id="rId1" display="http://www.nhs.uk/conditions/emollients/Pages/Introduction.aspx" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="C46" r:id="rId1" display="http://www.nhs.uk/conditions/emollients/Pages/Introduction.aspx" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Database is now on the final revision and is going into final testing.
</commit_message>
<xml_diff>
--- a/Entity Relationship Diagram/Database Data/Dummy Data.xlsx
+++ b/Entity Relationship Diagram/Database Data/Dummy Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitRepos\circle_lab_project\Entity Relationship Diagram\Database Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C224EAC7-60CD-4D8D-93DB-0DD5FA4778D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E38D015-EDD3-4885-8683-FA4C283E4281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{AED28F28-28A4-49FA-98A9-4DD437F4C446}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AED28F28-28A4-49FA-98A9-4DD437F4C446}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{528E7105-FF1C-4147-B82E-CE0932820990}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>